<commit_message>
added measurements doc and edited logic doc
</commit_message>
<xml_diff>
--- a/extra/universities.xlsx
+++ b/extra/universities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2FE1E5-5552-4F75-90A7-0393EC24EDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9BD68A-45E9-45A2-BCBD-45AFE9E446C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA721CF5-C791-44B2-8259-25B2876AE1CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA721CF5-C791-44B2-8259-25B2876AE1CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>university</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>application before finishing the third year?</t>
+  </si>
+  <si>
+    <t>ntnu?</t>
   </si>
 </sst>
 </file>
@@ -297,10 +300,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -520,8 +525,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AACF8C48-8F8D-4B1F-9B6A-40A8161B823B}" name="Tabella1" displayName="Tabella1" ref="A1:I22" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I22" xr:uid="{AACF8C48-8F8D-4B1F-9B6A-40A8161B823B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AACF8C48-8F8D-4B1F-9B6A-40A8161B823B}" name="Tabella1" displayName="Tabella1" ref="A1:I23" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I23" xr:uid="{AACF8C48-8F8D-4B1F-9B6A-40A8161B823B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
     <sortCondition ref="B1:B22"/>
   </sortState>
@@ -837,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E37745-C62F-49A0-9816-E5BBB48B8007}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="H20" sqref="H19:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +886,7 @@
       <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -910,7 +915,7 @@
       <c r="H2" s="3">
         <v>45031</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -937,7 +942,7 @@
       <c r="H3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -964,7 +969,7 @@
       <c r="H4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -991,7 +996,7 @@
       <c r="H5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1018,7 +1023,7 @@
       <c r="H6" s="3">
         <v>45031</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1045,7 +1050,7 @@
       <c r="H7" s="3">
         <v>45021</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1070,7 +1075,7 @@
         <v>69</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1093,7 +1098,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1118,7 +1123,7 @@
         <v>68</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1141,7 +1146,7 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1164,7 +1169,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1187,7 +1192,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="4"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1210,7 +1215,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="4"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1237,7 +1242,7 @@
       <c r="H15" s="3">
         <v>45044</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1264,7 +1269,7 @@
       <c r="H16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1291,7 +1296,7 @@
       <c r="H17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1318,7 +1323,7 @@
       <c r="H18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1345,7 +1350,7 @@
       <c r="H19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1372,7 +1377,7 @@
       <c r="H20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1399,7 +1404,7 @@
       <c r="H21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1426,7 +1431,20 @@
       <c r="H22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
added robotics, bioinformatics, reti logiche docs
</commit_message>
<xml_diff>
--- a/extra/universities.xlsx
+++ b/extra/universities.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9BD68A-45E9-45A2-BCBD-45AFE9E446C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB6FA9D-442D-4865-88AD-0DF8E53585AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA721CF5-C791-44B2-8259-25B2876AE1CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AA721CF5-C791-44B2-8259-25B2876AE1CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="all intersting uni" sheetId="1" r:id="rId1"/>
+    <sheet name="uni in sweden" sheetId="3" r:id="rId2"/>
+    <sheet name="possible uni" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
   <si>
     <t>university</t>
   </si>
@@ -39,15 +41,6 @@
     <t>ranking</t>
   </si>
   <si>
-    <t>eth</t>
-  </si>
-  <si>
-    <t>switzerland</t>
-  </si>
-  <si>
-    <t>zurich</t>
-  </si>
-  <si>
     <t>delft university of technology</t>
   </si>
   <si>
@@ -192,24 +185,15 @@
     <t>lund university</t>
   </si>
   <si>
-    <t>1 november - 15 december</t>
-  </si>
-  <si>
     <t>30 november - 2 january</t>
   </si>
   <si>
     <t>admission results publication</t>
   </si>
   <si>
-    <t>1 december - 3 january</t>
-  </si>
-  <si>
     <t>21 march</t>
   </si>
   <si>
-    <t>beginning of april</t>
-  </si>
-  <si>
     <t>16 october - 15 january</t>
   </si>
   <si>
@@ -237,17 +221,68 @@
     <t>attesa mail applicazione</t>
   </si>
   <si>
-    <t>application before finishing the third year?</t>
-  </si>
-  <si>
-    <t>ntnu?</t>
+    <t>ntnu</t>
+  </si>
+  <si>
+    <t>Gjøvik</t>
+  </si>
+  <si>
+    <t>may</t>
+  </si>
+  <si>
+    <t>1 February - 1 march</t>
+  </si>
+  <si>
+    <t>1 May - 15 June</t>
+  </si>
+  <si>
+    <t>university of hamburg</t>
+  </si>
+  <si>
+    <t>germany</t>
+  </si>
+  <si>
+    <t>hamburg</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>Computer and Systems Sciences</t>
+  </si>
+  <si>
+    <t>stuff to apply</t>
+  </si>
+  <si>
+    <t>motivation letter</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Software Engineering and Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">statement of purpose </t>
+  </si>
+  <si>
+    <t>(Machine Learning, Systems and Control)</t>
+  </si>
+  <si>
+    <t>(data science and AI)</t>
+  </si>
+  <si>
+    <t>software Engineering and technology</t>
+  </si>
+  <si>
+    <t>1 december - 16 january</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,18 +303,102 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF272833"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4E4E4E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4B4B4B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24273A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D4C44"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -289,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -300,36 +419,37 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -525,21 +645,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AACF8C48-8F8D-4B1F-9B6A-40A8161B823B}" name="Tabella1" displayName="Tabella1" ref="A1:I23" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I23" xr:uid="{AACF8C48-8F8D-4B1F-9B6A-40A8161B823B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
-    <sortCondition ref="B1:B22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AACF8C48-8F8D-4B1F-9B6A-40A8161B823B}" name="Tabella1" displayName="Tabella1" ref="A1:H23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H23" xr:uid="{AACF8C48-8F8D-4B1F-9B6A-40A8161B823B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H23">
+    <sortCondition ref="B1:B23"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{710196B2-2782-42EE-91E2-E6DCCF78B9A0}" name="university" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{AA9AA1C9-F1A7-4708-9250-52C57648BEA3}" name="country" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{7253189B-7999-4F51-A480-5E028BDE154C}" name="city" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{F9A03908-2EB3-47A7-880A-1028F985E5EF}" name="city pop (k)" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{FBAA1356-3C0D-4FE2-948A-CF9F0D9C848F}" name="ranking" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{300BEA3A-87E6-44B4-9087-6E8374B51987}" name="size" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{5768860C-7DB6-4D61-8B96-EC7584586ABE}" name="Application period" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{7C29A97F-FBEB-41DF-AE42-9680E0D391F7}" name="admission results publication" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{B086DC02-A821-4F9D-BA74-1878D49478C4}" name="application before finishing the third year?" dataDxfId="0"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{710196B2-2782-42EE-91E2-E6DCCF78B9A0}" name="university" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AA9AA1C9-F1A7-4708-9250-52C57648BEA3}" name="country" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{7253189B-7999-4F51-A480-5E028BDE154C}" name="city" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{F9A03908-2EB3-47A7-880A-1028F985E5EF}" name="city pop (k)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{FBAA1356-3C0D-4FE2-948A-CF9F0D9C848F}" name="ranking" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{300BEA3A-87E6-44B4-9087-6E8374B51987}" name="size" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{5768860C-7DB6-4D61-8B96-EC7584586ABE}" name="Application period" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{7C29A97F-FBEB-41DF-AE42-9680E0D391F7}" name="admission results publication" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -842,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E37745-C62F-49A0-9816-E5BBB48B8007}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H20" sqref="H19:H20"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,10 +977,9 @@
     <col min="6" max="6" width="7.140625" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -872,33 +990,30 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1">
         <v>656</v>
@@ -907,25 +1022,24 @@
         <v>121</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H2" s="3">
         <v>45031</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
         <v>656</v>
@@ -934,25 +1048,24 @@
         <v>107</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1">
         <v>285</v>
@@ -961,25 +1074,24 @@
         <v>143</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1">
         <v>221</v>
@@ -988,25 +1100,24 @@
         <v>336</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="1">
         <v>631</v>
@@ -1015,25 +1126,24 @@
         <v>115</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="H6" s="3">
         <v>45031</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>272</v>
@@ -1042,409 +1152,398 @@
         <v>109</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H7" s="3">
         <v>45021</v>
       </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1900</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1">
-        <v>921</v>
-      </c>
-      <c r="E8" s="1">
-        <v>53</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D9" s="1">
         <v>921</v>
       </c>
       <c r="E9" s="1">
+        <v>53</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>921</v>
+      </c>
+      <c r="E10" s="1">
         <v>207</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1">
         <v>358</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>107</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="F11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1">
         <v>223</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>124</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="1">
-        <v>158</v>
-      </c>
-      <c r="E12" s="1">
-        <v>210</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="D13" s="1">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="E13" s="1">
-        <v>126</v>
+        <v>210</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="E14" s="1">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>101</v>
+      </c>
+      <c r="E15" s="1">
+        <v>47</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1">
+        <v>702</v>
+      </c>
+      <c r="E16" s="1">
+        <v>117</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="3">
+        <v>45044</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1">
         <v>30</v>
       </c>
-      <c r="D15" s="1">
-        <v>702</v>
-      </c>
-      <c r="E15" s="1">
-        <v>117</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="3">
-        <v>45044</v>
-      </c>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="E17" s="1">
+        <v>264</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1">
         <v>984</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E18" s="1">
         <v>73</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="F18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1">
         <v>984</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E19" s="1">
         <v>118</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="F19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="1">
         <v>578</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E20" s="1">
         <v>187</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="F20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1">
         <v>578</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E21" s="1">
         <v>129</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="1">
-        <v>172</v>
-      </c>
-      <c r="E20" s="1">
-        <v>105</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="1">
-        <v>91</v>
-      </c>
-      <c r="E21" s="1">
-        <v>85</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D22" s="1">
-        <v>402</v>
+        <v>172</v>
       </c>
       <c r="E22" s="1">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1">
+        <v>91</v>
+      </c>
+      <c r="E23" s="1">
+        <v>85</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1454,4 +1553,208 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4CC763-9474-454A-8B63-B3712D76AF6B}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7">
+        <v>984</v>
+      </c>
+      <c r="D2" s="7">
+        <v>73</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7">
+        <v>984</v>
+      </c>
+      <c r="D3" s="7">
+        <v>118</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="7">
+        <v>578</v>
+      </c>
+      <c r="D4" s="7">
+        <v>187</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="7">
+        <v>578</v>
+      </c>
+      <c r="D6" s="7">
+        <v>129</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="7">
+        <v>172</v>
+      </c>
+      <c r="D8" s="7">
+        <v>105</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7">
+        <v>91</v>
+      </c>
+      <c r="D9" s="7">
+        <v>85</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A59D2A6-1FE2-49BC-AED3-2D04E7029C2E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated master uni docs
</commit_message>
<xml_diff>
--- a/extra/universities.xlsx
+++ b/extra/universities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B412887-BCAA-48E8-B243-5B086AD72051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F8EB79-A93B-4A03-9760-F4451B01DA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="-3435" windowWidth="38670" windowHeight="21150" xr2:uid="{AA721CF5-C791-44B2-8259-25B2876AE1CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA721CF5-C791-44B2-8259-25B2876AE1CF}"/>
   </bookViews>
   <sheets>
     <sheet name="all intersting uni" sheetId="1" r:id="rId1"/>
@@ -353,7 +353,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,6 +375,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,14 +472,16 @@
     <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1015,7 +1023,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:H11"/>
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,90 +1063,90 @@
       <c r="H1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="19">
         <v>656</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="19">
         <v>121</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="20">
         <v>45031</v>
       </c>
-      <c r="I2" s="17"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="17">
         <v>656</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="17">
         <v>107</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="17"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="17">
         <v>285</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="17">
         <v>143</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="17"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1165,7 +1173,7 @@
       <c r="H5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="17"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
@@ -1192,7 +1200,7 @@
       <c r="H6" s="16">
         <v>45031</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1221,7 +1229,7 @@
       <c r="H7" s="16">
         <v>45021</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1244,7 +1252,7 @@
         <v>68</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="17"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -1269,30 +1277,30 @@
         <v>63</v>
       </c>
       <c r="H9" s="15"/>
-      <c r="I9" s="17"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="17">
         <v>921</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="17">
         <v>207</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1317,7 +1325,7 @@
         <v>62</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="17"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1340,7 +1348,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="17"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1363,7 +1371,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="17"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1386,7 +1394,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="17"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1409,7 +1417,7 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="17"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1436,7 +1444,7 @@
       <c r="H16" s="3">
         <v>45044</v>
       </c>
-      <c r="I16" s="17"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1461,7 +1469,7 @@
       <c r="H17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I17" s="17"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
@@ -1488,115 +1496,115 @@
       <c r="H18" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="17"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="17">
         <v>984</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="17">
         <v>118</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="17"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="17">
         <v>578</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="17">
         <v>187</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="17"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="17">
         <v>578</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="17">
         <v>129</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="17"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="17">
         <v>172</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="17">
         <v>105</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="17"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -1623,7 +1631,7 @@
       <c r="H23" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="I23" s="17"/>
+      <c r="I23" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>